<commit_message>
New framework, scopewriter docs
</commit_message>
<xml_diff>
--- a/Documents/LCD Layout.xlsx
+++ b/Documents/LCD Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\scelbi-3-replica\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\scelbi-8-replica\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
   <si>
     <t>X</t>
   </si>
@@ -72,13 +72,28 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,18 +104,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,12 +143,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -403,98 +434,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="B1:U1"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <f>B1+1</f>
         <v>1</v>
       </c>
-      <c r="D1" s="2">
-        <f t="shared" ref="D1:Y1" si="0">C1+1</f>
+      <c r="D1" s="3">
+        <f t="shared" ref="D1:U1" si="0">C1+1</f>
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
@@ -540,7 +571,7 @@
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -595,7 +626,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -646,7 +677,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -688,6 +719,275 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <f>B7+1</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ref="D7" si="1">C7+1</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" ref="E7" si="2">D7+1</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ref="F7" si="3">E7+1</f>
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7" si="4">F7+1</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" ref="H7" si="5">G7+1</f>
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" ref="I7" si="6">H7+1</f>
+        <v>7</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" ref="J7" si="7">I7+1</f>
+        <v>8</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" ref="K7" si="8">J7+1</f>
+        <v>9</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" ref="L7" si="9">K7+1</f>
+        <v>10</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" ref="M7" si="10">L7+1</f>
+        <v>11</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" ref="N7" si="11">M7+1</f>
+        <v>12</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" ref="O7" si="12">N7+1</f>
+        <v>13</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" ref="P7" si="13">O7+1</f>
+        <v>14</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" ref="Q7" si="14">P7+1</f>
+        <v>15</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" ref="R7" si="15">Q7+1</f>
+        <v>16</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" ref="S7" si="16">R7+1</f>
+        <v>17</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" ref="T7" si="17">S7+1</f>
+        <v>18</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" ref="U7" si="18">T7+1</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>